<commit_message>
scripts and dll added
</commit_message>
<xml_diff>
--- a/Application_Tier/PageObjectRepository/ApplicantPortal/Applicant_Portal_Details.xlsx
+++ b/Application_Tier/PageObjectRepository/ApplicantPortal/Applicant_Portal_Details.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>DOB</t>
   </si>
@@ -30,7 +30,22 @@
     <t>ChickName</t>
   </si>
   <si>
+    <t>Test Automation</t>
+  </si>
+  <si>
+    <t>28/10/2019</t>
+  </si>
+  <si>
     <t>Y000-102-01</t>
+  </si>
+  <si>
+    <t>24/11/2019</t>
+  </si>
+  <si>
+    <t>M000-097-01</t>
+  </si>
+  <si>
+    <t>T000-105-01</t>
   </si>
 </sst>
 </file>
@@ -74,9 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,16 +373,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" activeCellId="3" sqref="A2 B4 B3 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="40.36328125" customWidth="1"/>
+    <col min="2" max="2" width="42.1796875" customWidth="1"/>
     <col min="3" max="3" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -385,6 +401,56 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42928</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>